<commit_message>
co chinh phan xuat
</commit_message>
<xml_diff>
--- a/upload/KE HOACH GIANG DAY Tin UD K42.xlsx
+++ b/upload/KE HOACH GIANG DAY Tin UD K42.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tin học UD K42'!$A$1:$J$83</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -31,12 +31,6 @@
     <t>Độc lập - Tự do - Hạnh phúc</t>
   </si>
   <si>
-    <t>KẾ HOẠCH GIẢNG DẠY HỆ CAO ĐẲNG - KHÓA 42</t>
-  </si>
-  <si>
-    <t>Khóa học 42 (2017-2020)</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
@@ -157,19 +151,6 @@
   </si>
   <si>
     <t>Anh văn 2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">HỌC KỲ IV: ……16…….. TC/ĐVHT </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(Bắt buộc: ……16…….TC/ ĐVHT, Tự chọn:…0…… TC/ ĐVHT)</t>
-    </r>
   </si>
   <si>
     <t>Cần Thơ, ngày 21 tháng 12 năm 2017</t>
@@ -393,6 +374,25 @@
   </si>
   <si>
     <t>Lập trình truyền  thông</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HỌC KỲ IV: ……16…….. TC/ĐVHT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Bắt buộc: ……16…….TC/ ĐVHT, Tự chọn:…4…… TC/ ĐVHT)</t>
+    </r>
+  </si>
+  <si>
+    <t>Khóa học 42 (2017-2020)</t>
+  </si>
+  <si>
+    <t>KẾ HOẠCH GIẢNG DẠY HỆ CAO ĐẲNG - KHÓA 42</t>
   </si>
 </sst>
 </file>
@@ -632,35 +632,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,8 +1061,8 @@
   </sheetPr>
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1078,125 +1078,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="E2" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="E2" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+      <c r="A4" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
     </row>
     <row r="5" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
+      <c r="A5" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="A6" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
+      <c r="A8" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
     </row>
     <row r="10" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
@@ -1204,16 +1204,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="13">
         <v>2</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="11">
@@ -1234,14 +1234,14 @@
         <v>2</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="11">
@@ -1262,14 +1262,14 @@
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="11">
@@ -1290,16 +1290,16 @@
         <v>4</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>54</v>
-      </c>
       <c r="D14" s="13">
         <v>3</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="11">
@@ -1320,16 +1320,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D15" s="11">
         <v>2</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11">
@@ -1350,16 +1350,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="13">
         <v>3</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="11">
@@ -1380,16 +1380,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" s="11">
         <v>3</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="11">
@@ -1410,16 +1410,16 @@
         <v>8</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="11">
         <v>3</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="11">
@@ -1440,16 +1440,16 @@
         <v>9</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D19" s="15">
         <v>2</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="11">
@@ -1466,11 +1466,11 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="16">
         <f>SUM(D11:D19)</f>
         <v>18</v>
@@ -1507,49 +1507,49 @@
       <c r="J21" s="18"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
+      <c r="A22" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
@@ -1557,16 +1557,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" s="13">
         <v>2</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="11">
@@ -1587,14 +1587,14 @@
         <v>2</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="11">
@@ -1615,16 +1615,16 @@
         <v>3</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D27" s="13">
         <v>3</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="11">
@@ -1645,14 +1645,14 @@
         <v>4</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="11">
@@ -1673,16 +1673,16 @@
         <v>5</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D29" s="11">
         <v>3</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="11">
@@ -1703,16 +1703,16 @@
         <v>6</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D30" s="11">
         <v>2</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="11">
@@ -1733,16 +1733,16 @@
         <v>7</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D31" s="11">
         <v>3</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="11">
@@ -1763,16 +1763,16 @@
         <v>8</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D32" s="11">
         <v>3</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="11">
@@ -1793,14 +1793,14 @@
         <v>9</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="11">
@@ -1817,11 +1817,11 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A34" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
       <c r="D34" s="16">
         <f>SUM(D25:D32)</f>
         <v>16</v>
@@ -1853,49 +1853,49 @@
     </row>
     <row r="35" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
+      <c r="A36" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
     </row>
     <row r="38" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="D38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="E38" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="G38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="H38" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="I38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="J38" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1903,16 +1903,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D39" s="11">
         <v>3</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="11">
@@ -1933,16 +1933,16 @@
         <v>2</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D40" s="11">
         <v>3</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="11">
@@ -1963,16 +1963,16 @@
         <v>3</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D41" s="11">
         <v>3</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="11">
@@ -1993,16 +1993,16 @@
         <v>4</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D42" s="11">
         <v>3</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="11">
@@ -2023,16 +2023,16 @@
         <v>5</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D43" s="11">
         <v>3</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="11">
@@ -2053,14 +2053,14 @@
         <v>6</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="11">
@@ -2077,11 +2077,11 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
+      <c r="A45" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
       <c r="D45" s="16">
         <f>SUM(D39:D43)</f>
         <v>15</v>
@@ -2112,49 +2112,49 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
+      <c r="A47" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
     </row>
     <row r="49" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="D49" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="E49" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="F49" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="G49" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="H49" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="I49" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="J49" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2162,16 +2162,16 @@
         <v>1</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D50" s="11">
         <v>1</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="11">
@@ -2192,16 +2192,16 @@
         <v>2</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D51" s="11">
         <v>3</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="11">
@@ -2222,16 +2222,16 @@
         <v>3</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D52" s="11">
         <v>3</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="11">
@@ -2252,16 +2252,16 @@
         <v>4</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D53" s="11">
         <v>3</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="11">
@@ -2282,16 +2282,16 @@
         <v>5</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D54" s="11">
         <v>3</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="11">
@@ -2312,16 +2312,16 @@
         <v>6</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D55" s="11">
         <v>3</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="11">
@@ -2342,14 +2342,14 @@
         <v>7</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D56" s="11"/>
       <c r="E56" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="11">
@@ -2366,11 +2366,11 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A57" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
+      <c r="A57" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
       <c r="D57" s="19">
         <f>SUM(D50:D55)</f>
         <v>16</v>
@@ -2401,49 +2401,49 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
-      <c r="J59" s="32"/>
+      <c r="A59" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="33"/>
     </row>
     <row r="61" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="D61" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="E61" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="F61" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="G61" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="H61" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="5" t="s">
+      <c r="I61" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="J61" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="I61" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2451,17 +2451,17 @@
         <v>1</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D62" s="11">
         <v>1</v>
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G62" s="11">
         <v>45</v>
@@ -2481,16 +2481,16 @@
         <v>2</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D63" s="11">
         <v>3</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="11">
@@ -2511,16 +2511,16 @@
         <v>3</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D64" s="11">
         <v>2</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="11">
@@ -2541,16 +2541,16 @@
         <v>4</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D65" s="11">
         <v>2</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="11">
@@ -2571,14 +2571,14 @@
         <v>5</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D66" s="23"/>
       <c r="E66" s="24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F66" s="24"/>
       <c r="G66" s="23">
@@ -2597,21 +2597,21 @@
       </c>
     </row>
     <row r="67" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="33">
+      <c r="A67" s="35">
         <v>6</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D67" s="11">
         <v>2</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G67" s="11">
         <v>45</v>
@@ -2627,19 +2627,19 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="34"/>
+      <c r="A68" s="36"/>
       <c r="B68" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D68" s="11">
         <v>2</v>
       </c>
       <c r="E68" s="10"/>
       <c r="F68" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G68" s="11">
         <v>45</v>
@@ -2655,19 +2655,19 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
+      <c r="A69" s="36"/>
       <c r="B69" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D69" s="11">
         <v>2</v>
       </c>
       <c r="E69" s="10"/>
       <c r="F69" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G69" s="11">
         <v>45</v>
@@ -2683,19 +2683,19 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="34"/>
+      <c r="A70" s="36"/>
       <c r="B70" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D70" s="11">
         <v>2</v>
       </c>
       <c r="E70" s="10"/>
       <c r="F70" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G70" s="11">
         <v>45</v>
@@ -2711,19 +2711,19 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
+      <c r="A71" s="36"/>
       <c r="B71" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D71" s="11">
         <v>2</v>
       </c>
       <c r="E71" s="10"/>
       <c r="F71" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G71" s="11">
         <v>45</v>
@@ -2739,19 +2739,19 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+      <c r="A72" s="36"/>
       <c r="B72" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D72" s="11">
         <v>2</v>
       </c>
       <c r="E72" s="10"/>
       <c r="F72" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G72" s="11">
         <v>45</v>
@@ -2767,11 +2767,11 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A73" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="28"/>
-      <c r="C73" s="28"/>
+      <c r="A73" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
       <c r="D73" s="25">
         <f>SUM(D62:D67)</f>
         <v>10</v>
@@ -2837,48 +2837,41 @@
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
-      <c r="G78" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="H78" s="29"/>
-      <c r="I78" s="29"/>
-      <c r="J78" s="29"/>
+      <c r="G78" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="37"/>
     </row>
     <row r="79" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B79" s="30"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="E79" s="30"/>
-      <c r="F79" s="30"/>
-      <c r="G79" s="30" t="s">
+      <c r="A79" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B79" s="28"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E79" s="28"/>
+      <c r="F79" s="28"/>
+      <c r="G79" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H79" s="30"/>
-      <c r="I79" s="30"/>
-      <c r="J79" s="30"/>
+      <c r="H79" s="28"/>
+      <c r="I79" s="28"/>
+      <c r="J79" s="28"/>
     </row>
     <row r="82" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B83" s="30"/>
-      <c r="C83" s="30"/>
+      <c r="A83" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="A4:J4"/>
     <mergeCell ref="A83:C83"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A8:J8"/>
@@ -2895,6 +2888,13 @@
     <mergeCell ref="G78:J78"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="D79:F79"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="A4:J4"/>
     <mergeCell ref="G79:J79"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>